<commit_message>
Update PM11 Tidsregistrering for Rasmus.xlsx
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM11 Tidsregistrering for Rasmus.xlsx
+++ b/08 Project Management/Tidsregistrering/PM11 Tidsregistrering for Rasmus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rasmus J\Documents\GitHub\HoeKulator\08 Project Management\Tidsregistrering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rasmus J\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E360B9C-9212-4627-B0F2-C2E8FFD72BBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E2A8A2D-14EC-4793-AC3F-806D8404F899}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23258" windowHeight="12578" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>Tidsregistrering af (Navn)</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>30 minutter</t>
+  </si>
+  <si>
+    <t>Viderearbejde med mockup</t>
   </si>
 </sst>
 </file>
@@ -758,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -924,17 +927,31 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="19.5" x14ac:dyDescent="0.6">
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="19"/>
+      <c r="A7" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="13">
+        <v>43886</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0.4375</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>46</v>
+      </c>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.6388888888888895E-2</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(G$3:G7)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -948,7 +965,7 @@
       </c>
       <c r="H8" s="1">
         <f>SUM(G$3:G8)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -962,7 +979,7 @@
       </c>
       <c r="H9" s="1">
         <f>SUM(G$3:G9)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -976,7 +993,7 @@
       </c>
       <c r="H10" s="1">
         <f>SUM(G$3:G10)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -990,7 +1007,7 @@
       </c>
       <c r="H11" s="1">
         <f>SUM(G$3:G11)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1004,7 +1021,7 @@
       </c>
       <c r="H12" s="1">
         <f>SUM(G$3:G12)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1018,7 +1035,7 @@
       </c>
       <c r="H13" s="1">
         <f>SUM(G$3:G13)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1030,7 +1047,7 @@
       </c>
       <c r="H14" s="1">
         <f>SUM(G$3:G14)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1042,7 +1059,7 @@
       </c>
       <c r="H15" s="1">
         <f>SUM(G$3:G15)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1054,7 +1071,7 @@
       </c>
       <c r="H16" s="1">
         <f>SUM(G$3:G16)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1066,7 +1083,7 @@
       </c>
       <c r="H17" s="1">
         <f>SUM(G$3:G17)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1078,7 +1095,7 @@
       </c>
       <c r="H18" s="1">
         <f>SUM(G$3:G18)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1090,7 +1107,7 @@
       </c>
       <c r="H19" s="1">
         <f>SUM(G$3:G19)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1102,7 +1119,7 @@
       </c>
       <c r="H20" s="1">
         <f>SUM(G$3:G20)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1114,7 +1131,7 @@
       </c>
       <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1126,7 +1143,7 @@
       </c>
       <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1138,7 +1155,7 @@
       </c>
       <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1150,7 +1167,7 @@
       </c>
       <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1161,7 +1178,7 @@
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1172,7 +1189,7 @@
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1183,7 +1200,7 @@
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1194,7 +1211,7 @@
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1205,7 +1222,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1216,7 +1233,7 @@
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="31" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1227,7 +1244,7 @@
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="19.5" x14ac:dyDescent="0.6">
@@ -1238,7 +1255,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>0.22222222222222227</v>
+        <v>0.29861111111111116</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.45">

</xml_diff>